<commit_message>
OTP sent to mobile as well as email, updated database as well
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shreyash\OneDrive\Desktop\task1\module1 [dated 03.01.2025]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFDE081-3BB2-4916-9D3D-FC8425222DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243D738B-4BEA-4A3B-AC17-9424768B3C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="146">
   <si>
     <t>name</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>phone_no</t>
   </si>
 </sst>
 </file>
@@ -786,21 +789,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -816,8 +820,11 @@
       <c r="E1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -833,8 +840,11 @@
       <c r="E2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -850,8 +860,11 @@
       <c r="E3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2300</v>
       </c>
@@ -867,8 +880,11 @@
       <c r="E4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>7387256694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2301</v>
       </c>
@@ -884,8 +900,11 @@
       <c r="E5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2302</v>
       </c>
@@ -901,8 +920,12 @@
       <c r="E6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" ref="F6:F69" si="0">F5+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2303</v>
       </c>
@@ -918,8 +941,12 @@
       <c r="E7" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2304</v>
       </c>
@@ -935,8 +962,12 @@
       <c r="E8" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2305</v>
       </c>
@@ -952,8 +983,12 @@
       <c r="E9" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2306</v>
       </c>
@@ -969,8 +1004,12 @@
       <c r="E10" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2307</v>
       </c>
@@ -986,8 +1025,12 @@
       <c r="E11" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2308</v>
       </c>
@@ -1003,8 +1046,12 @@
       <c r="E12" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2309</v>
       </c>
@@ -1020,8 +1067,12 @@
       <c r="E13" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2311</v>
       </c>
@@ -1037,8 +1088,12 @@
       <c r="E14" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2313</v>
       </c>
@@ -1054,8 +1109,12 @@
       <c r="E15" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2314</v>
       </c>
@@ -1071,8 +1130,12 @@
       <c r="E16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2315</v>
       </c>
@@ -1088,8 +1151,12 @@
       <c r="E17" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2316</v>
       </c>
@@ -1105,8 +1172,12 @@
       <c r="E18" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2317</v>
       </c>
@@ -1122,8 +1193,12 @@
       <c r="E19" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2318</v>
       </c>
@@ -1139,8 +1214,12 @@
       <c r="E20" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2319</v>
       </c>
@@ -1156,8 +1235,12 @@
       <c r="E21" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2320</v>
       </c>
@@ -1173,8 +1256,12 @@
       <c r="E22" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2321</v>
       </c>
@@ -1190,8 +1277,12 @@
       <c r="E23" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2322</v>
       </c>
@@ -1207,8 +1298,12 @@
       <c r="E24" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2323</v>
       </c>
@@ -1224,8 +1319,12 @@
       <c r="E25" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2324</v>
       </c>
@@ -1241,8 +1340,12 @@
       <c r="E26" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2325</v>
       </c>
@@ -1258,8 +1361,12 @@
       <c r="E27" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2326</v>
       </c>
@@ -1275,8 +1382,12 @@
       <c r="E28" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2327</v>
       </c>
@@ -1292,8 +1403,12 @@
       <c r="E29" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2328</v>
       </c>
@@ -1309,8 +1424,12 @@
       <c r="E30" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2329</v>
       </c>
@@ -1326,8 +1445,12 @@
       <c r="E31" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2330</v>
       </c>
@@ -1343,8 +1466,12 @@
       <c r="E32" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2331</v>
       </c>
@@ -1360,8 +1487,12 @@
       <c r="E33" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2333</v>
       </c>
@@ -1377,8 +1508,12 @@
       <c r="E34" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2334</v>
       </c>
@@ -1394,8 +1529,12 @@
       <c r="E35" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2335</v>
       </c>
@@ -1411,8 +1550,12 @@
       <c r="E36" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2336</v>
       </c>
@@ -1428,8 +1571,12 @@
       <c r="E37" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2337</v>
       </c>
@@ -1445,8 +1592,12 @@
       <c r="E38" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2338</v>
       </c>
@@ -1462,8 +1613,12 @@
       <c r="E39" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2339</v>
       </c>
@@ -1479,8 +1634,12 @@
       <c r="E40" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2340</v>
       </c>
@@ -1496,8 +1655,12 @@
       <c r="E41" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2341</v>
       </c>
@@ -1513,8 +1676,12 @@
       <c r="E42" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2342</v>
       </c>
@@ -1530,8 +1697,12 @@
       <c r="E43" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2344</v>
       </c>
@@ -1547,8 +1718,12 @@
       <c r="E44" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2345</v>
       </c>
@@ -1564,8 +1739,12 @@
       <c r="E45" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2346</v>
       </c>
@@ -1581,8 +1760,12 @@
       <c r="E46" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2348</v>
       </c>
@@ -1598,8 +1781,12 @@
       <c r="E47" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2350</v>
       </c>
@@ -1615,8 +1802,12 @@
       <c r="E48" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2352</v>
       </c>
@@ -1632,8 +1823,12 @@
       <c r="E49" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2353</v>
       </c>
@@ -1649,8 +1844,12 @@
       <c r="E50" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2354</v>
       </c>
@@ -1666,8 +1865,12 @@
       <c r="E51" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2355</v>
       </c>
@@ -1683,8 +1886,12 @@
       <c r="E52" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2356</v>
       </c>
@@ -1700,8 +1907,12 @@
       <c r="E53" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2357</v>
       </c>
@@ -1717,8 +1928,12 @@
       <c r="E54" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2358</v>
       </c>
@@ -1734,8 +1949,12 @@
       <c r="E55" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2359</v>
       </c>
@@ -1751,8 +1970,12 @@
       <c r="E56" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2360</v>
       </c>
@@ -1768,8 +1991,12 @@
       <c r="E57" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2361</v>
       </c>
@@ -1785,8 +2012,12 @@
       <c r="E58" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2362</v>
       </c>
@@ -1802,8 +2033,12 @@
       <c r="E59" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2363</v>
       </c>
@@ -1819,8 +2054,12 @@
       <c r="E60" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2364</v>
       </c>
@@ -1836,8 +2075,12 @@
       <c r="E61" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2365</v>
       </c>
@@ -1853,8 +2096,12 @@
       <c r="E62" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2366</v>
       </c>
@@ -1870,8 +2117,12 @@
       <c r="E63" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2367</v>
       </c>
@@ -1887,8 +2138,12 @@
       <c r="E64" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2368</v>
       </c>
@@ -1904,8 +2159,12 @@
       <c r="E65" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2369</v>
       </c>
@@ -1921,8 +2180,12 @@
       <c r="E66" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2370</v>
       </c>
@@ -1938,8 +2201,12 @@
       <c r="E67" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2371</v>
       </c>
@@ -1955,8 +2222,12 @@
       <c r="E68" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2372</v>
       </c>
@@ -1972,8 +2243,12 @@
       <c r="E69" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2374</v>
       </c>
@@ -1988,6 +2263,10 @@
       </c>
       <c r="E70" t="s">
         <v>143</v>
+      </c>
+      <c r="F70">
+        <f t="shared" ref="F70" si="1">F69+1</f>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit for ram to do remaining work!!!!
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shreyash\OneDrive\Desktop\task1\module1 [dated 03.01.2025]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243D738B-4BEA-4A3B-AC17-9424768B3C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1832F12-525D-4D9B-A882-A0CF8899DD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,6 +478,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;+91&quot;#"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -507,8 +510,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,22 +793,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
     <col min="8" max="8" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -824,7 +828,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -840,11 +844,11 @@
       <c r="E2" t="s">
         <v>144</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -860,11 +864,11 @@
       <c r="E3" t="s">
         <v>144</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2300</v>
       </c>
@@ -880,11 +884,12 @@
       <c r="E4" t="s">
         <v>144</v>
       </c>
-      <c r="F4">
-        <v>7387256694</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>8446872705</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2301</v>
       </c>
@@ -900,11 +905,11 @@
       <c r="E5" t="s">
         <v>143</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2302</v>
       </c>
@@ -920,12 +925,12 @@
       <c r="E6" t="s">
         <v>143</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <f t="shared" ref="F6:F69" si="0">F5+1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2303</v>
       </c>
@@ -941,12 +946,12 @@
       <c r="E7" t="s">
         <v>143</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2304</v>
       </c>
@@ -962,12 +967,12 @@
       <c r="E8" t="s">
         <v>143</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2305</v>
       </c>
@@ -983,12 +988,12 @@
       <c r="E9" t="s">
         <v>143</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2306</v>
       </c>
@@ -1004,12 +1009,12 @@
       <c r="E10" t="s">
         <v>143</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2307</v>
       </c>
@@ -1025,12 +1030,12 @@
       <c r="E11" t="s">
         <v>143</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2308</v>
       </c>
@@ -1046,12 +1051,12 @@
       <c r="E12" t="s">
         <v>143</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2309</v>
       </c>
@@ -1067,12 +1072,12 @@
       <c r="E13" t="s">
         <v>143</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2311</v>
       </c>
@@ -1088,12 +1093,12 @@
       <c r="E14" t="s">
         <v>143</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2313</v>
       </c>
@@ -1109,12 +1114,12 @@
       <c r="E15" t="s">
         <v>143</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2314</v>
       </c>
@@ -1130,7 +1135,7 @@
       <c r="E16" t="s">
         <v>143</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1151,7 +1156,7 @@
       <c r="E17" t="s">
         <v>143</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -1172,7 +1177,7 @@
       <c r="E18" t="s">
         <v>143</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1193,7 +1198,7 @@
       <c r="E19" t="s">
         <v>143</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1214,7 +1219,7 @@
       <c r="E20" t="s">
         <v>143</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1235,7 +1240,7 @@
       <c r="E21" t="s">
         <v>143</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1256,7 +1261,7 @@
       <c r="E22" t="s">
         <v>143</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1277,7 +1282,7 @@
       <c r="E23" t="s">
         <v>143</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -1298,7 +1303,7 @@
       <c r="E24" t="s">
         <v>143</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1319,7 +1324,7 @@
       <c r="E25" t="s">
         <v>143</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -1340,7 +1345,7 @@
       <c r="E26" t="s">
         <v>143</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -1361,7 +1366,7 @@
       <c r="E27" t="s">
         <v>143</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -1382,7 +1387,7 @@
       <c r="E28" t="s">
         <v>143</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -1403,7 +1408,7 @@
       <c r="E29" t="s">
         <v>143</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1424,7 +1429,7 @@
       <c r="E30" t="s">
         <v>143</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -1445,7 +1450,7 @@
       <c r="E31" t="s">
         <v>143</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -1466,7 +1471,7 @@
       <c r="E32" t="s">
         <v>143</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -1487,7 +1492,7 @@
       <c r="E33" t="s">
         <v>143</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
@@ -1508,7 +1513,7 @@
       <c r="E34" t="s">
         <v>143</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1529,7 +1534,7 @@
       <c r="E35" t="s">
         <v>143</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
@@ -1550,7 +1555,7 @@
       <c r="E36" t="s">
         <v>143</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -1571,7 +1576,7 @@
       <c r="E37" t="s">
         <v>143</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
@@ -1592,7 +1597,7 @@
       <c r="E38" t="s">
         <v>143</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
@@ -1613,7 +1618,7 @@
       <c r="E39" t="s">
         <v>143</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1634,7 +1639,7 @@
       <c r="E40" t="s">
         <v>143</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -1655,7 +1660,7 @@
       <c r="E41" t="s">
         <v>143</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
@@ -1676,7 +1681,7 @@
       <c r="E42" t="s">
         <v>143</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
@@ -1697,7 +1702,7 @@
       <c r="E43" t="s">
         <v>143</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
@@ -1718,7 +1723,7 @@
       <c r="E44" t="s">
         <v>143</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -1739,7 +1744,7 @@
       <c r="E45" t="s">
         <v>143</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
@@ -1760,7 +1765,7 @@
       <c r="E46" t="s">
         <v>143</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
@@ -1781,7 +1786,7 @@
       <c r="E47" t="s">
         <v>143</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
@@ -1802,7 +1807,7 @@
       <c r="E48" t="s">
         <v>143</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
@@ -1823,7 +1828,7 @@
       <c r="E49" t="s">
         <v>143</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
@@ -1844,7 +1849,7 @@
       <c r="E50" t="s">
         <v>143</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
@@ -1865,7 +1870,7 @@
       <c r="E51" t="s">
         <v>143</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
@@ -1886,7 +1891,7 @@
       <c r="E52" t="s">
         <v>143</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
@@ -1907,7 +1912,7 @@
       <c r="E53" t="s">
         <v>143</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
@@ -1928,7 +1933,7 @@
       <c r="E54" t="s">
         <v>143</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -1949,7 +1954,7 @@
       <c r="E55" t="s">
         <v>143</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="1">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
@@ -1970,7 +1975,7 @@
       <c r="E56" t="s">
         <v>143</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="1">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
@@ -1991,7 +1996,7 @@
       <c r="E57" t="s">
         <v>143</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="1">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
@@ -2012,7 +2017,7 @@
       <c r="E58" t="s">
         <v>143</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="1">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
@@ -2033,7 +2038,7 @@
       <c r="E59" t="s">
         <v>143</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
@@ -2054,7 +2059,7 @@
       <c r="E60" t="s">
         <v>143</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="1">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
@@ -2075,7 +2080,7 @@
       <c r="E61" t="s">
         <v>143</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="1">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
@@ -2096,7 +2101,7 @@
       <c r="E62" t="s">
         <v>143</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="1">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
@@ -2117,7 +2122,7 @@
       <c r="E63" t="s">
         <v>143</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
@@ -2138,7 +2143,7 @@
       <c r="E64" t="s">
         <v>143</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -2159,7 +2164,7 @@
       <c r="E65" t="s">
         <v>143</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="1">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
@@ -2180,7 +2185,7 @@
       <c r="E66" t="s">
         <v>143</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="1">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
@@ -2201,7 +2206,7 @@
       <c r="E67" t="s">
         <v>143</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="1">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
@@ -2222,7 +2227,7 @@
       <c r="E68" t="s">
         <v>143</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
@@ -2243,7 +2248,7 @@
       <c r="E69" t="s">
         <v>143</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="1">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
@@ -2264,17 +2269,18 @@
       <c r="E70" t="s">
         <v>143</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="1">
         <f t="shared" ref="F70" si="1">F69+1</f>
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Validation" error="Enter Valid Email Address" promptTitle="Enter Valid Email Address" prompt="Enter Valid Email Address" sqref="C25:C28 C31 C37:C38 C41 C46 C50 C52 C57:C58 C66:C70 I5:I65" xr:uid="{E619BEA3-04D1-4300-B9AA-7B77B18E1B6E}">
       <formula1>AND(ISERROR(FIND(" ",C5)),LEN(C5)-LEN(SUBSTITUTE(C5,"@",""))=1,IFERROR(SEARCH("@",C5)&lt;SEARCH(".",C5,SEARCH("@",C5)),0),NOT(IFERROR(SEARCH("@",C5),0)=1),NOT(IFERROR(SEARCH(".",C5,SEARCH("@",C5))-SEARCH("@",C5),0)=1),LEFT(C5,1)&lt;&gt;".",RIGHT(C5,1)&lt;&gt;".")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>